<commit_message>
feat: Update excel sheet to conform to new GRASP input
</commit_message>
<xml_diff>
--- a/base_files/GRASP_general.xlsx
+++ b/base_files/GRASP_general.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,54 +20,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>General Reaction and Sampling Platform (GRASP)</t>
-  </si>
-  <si>
-    <t>Model name</t>
-  </si>
-  <si>
-    <t>Sampling mode (ORACLE, rejection, rejectionSMC, SMC, MCMC-SMC)</t>
-  </si>
-  <si>
-    <t>ORACLE</t>
-  </si>
-  <si>
-    <t>NLP solver (NLOPT, OPTI, FMINCON (default))</t>
-  </si>
-  <si>
-    <t>FMINCON</t>
-  </si>
-  <si>
-    <t>Number of exp. conditions (excluding reference state)</t>
-  </si>
-  <si>
-    <t>Number of model structures</t>
-  </si>
-  <si>
-    <t>Number of particles</t>
-  </si>
-  <si>
-    <t>Parallel mode (ON = 1; OFF = 0)</t>
-  </si>
-  <si>
-    <t>Number of cores (ignored if Parallel mode disabled)</t>
-  </si>
-  <si>
-    <t>Percentile of alive particles for SMC (e.g., 20, 50, etc.) (only needed for rejectionSMC, SMC, MCMC-SMC)</t>
-  </si>
-  <si>
-    <t>Compute robust fluxes (ON = 1; OFF = 0)</t>
-  </si>
-  <si>
-    <t>Compute thermodynamics (ON = 1; OFF = 0)</t>
-  </si>
-  <si>
-    <t>Inicial tolerance (OPTIONAL)</t>
-  </si>
-  <si>
-    <t>Final tolerance (in the case of ORACLE, set to 1)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t xml:space="preserve">General Reaction and Sampling Platform (GRASP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sampling mode (GRASP or rejection)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRASP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLP solver (NLOPT or FMINCON (default))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMINCON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LP solver (linprog or gurobi)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gurobi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of exp. conditions (excluding reference state)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of model structures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parallel mode (ON = 1; OFF = 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of cores (ignored if Parallel mode disabled)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compute robust fluxes (ON = 1; OFF = 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final tolerance (in the case of GRASP, set to 1)</t>
   </si>
 </sst>
 </file>
@@ -75,7 +72,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -158,9 +155,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -184,30 +185,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.9068825910931"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.1093117408907"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="57.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.57"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="1" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -215,7 +217,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -223,84 +225,76 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="0" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
chore: Update base file
</commit_message>
<xml_diff>
--- a/base_files/GRASP_general.xlsx
+++ b/base_files/GRASP_general.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t xml:space="preserve">General Reaction and Sampling Platform (GRASP)</t>
   </si>
@@ -44,6 +44,15 @@
   </si>
   <si>
     <t xml:space="preserve">gurobi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prior distribution for fluxes (uniform or normal)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prior distribution for thermodynamic quantities (uniform or normal)</t>
   </si>
   <si>
     <t xml:space="preserve">Number of exp. conditions (excluding reference state)</t>
@@ -188,7 +197,7 @@
   <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="A11:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -237,55 +246,71 @@
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="0" t="n">
-        <v>0</v>
+      <c r="B6" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>9</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="0" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>